<commit_message>
new measures for ulinær system og oprydning
</commit_message>
<xml_diff>
--- a/CSV/MeasDataNewCalc.xlsx
+++ b/CSV/MeasDataNewCalc.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ditte\aauRepo\esd7_git\3Dprinter-BLDC-control\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B49EBAF8-83A3-4876-BAF0-8A21F63DB33B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{702EC506-C491-4E17-9D7B-6E4368C7C725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{1C1EA20F-3530-4221-A012-E83695529858}"/>
   </bookViews>
   <sheets>
     <sheet name="MeasDataNew" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>time(us)</t>
   </si>
@@ -32,6 +45,12 @@
   </si>
   <si>
     <t>rad/s</t>
+  </si>
+  <si>
+    <t>timeStamp</t>
+  </si>
+  <si>
+    <t>i</t>
   </si>
 </sst>
 </file>
@@ -628,6 +647,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MeasDataNew!$F$137</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rad/s</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="38100" cap="rnd">
               <a:noFill/>
@@ -652,55 +682,70 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>MeasDataNew!$D$138:$D$149</c:f>
+              <c:f>MeasDataNew!$E$138:$E$154</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3022219999999999E-2</c:v>
+                  <c:v>2.0414000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.6064644999999997E-2</c:v>
+                  <c:v>4.0619000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.9127257999999998E-2</c:v>
+                  <c:v>6.0807E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.2210056999999997E-2</c:v>
+                  <c:v>8.0992999999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.5313029999999994E-2</c:v>
+                  <c:v>0.10116699999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.8436189999999989E-2</c:v>
+                  <c:v>0.12135399999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.1579577999999995E-2</c:v>
+                  <c:v>0.14158199999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.10474317399999999</c:v>
+                  <c:v>0.16178999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.11792694299999999</c:v>
+                  <c:v>0.18196299999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.131130892</c:v>
+                  <c:v>0.20214299999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.144355021</c:v>
+                  <c:v>0.22232299999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.242503</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.26272299999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.28290399999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.30311399999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.32329399999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>MeasDataNew!$E$138:$E$149</c:f>
+              <c:f>MeasDataNew!$F$138:$F$154</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -734,13 +779,28 @@
                 <c:pt idx="11">
                   <c:v>12.804311999999999</c:v>
                 </c:pt>
+                <c:pt idx="12">
+                  <c:v>15.555652</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10.423332</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13.227606</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>13.386321000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>13.386333</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-ABC1-4E0D-9CA0-46F8D88B59C2}"/>
+              <c16:uniqueId val="{00000000-30F1-4CCA-8D68-A7FD497B4953}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -752,11 +812,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="49871935"/>
-        <c:axId val="49872895"/>
+        <c:axId val="1185549407"/>
+        <c:axId val="1185549887"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="49871935"/>
+        <c:axId val="1185549407"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -813,12 +873,12 @@
             <a:endParaRPr lang="en-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49872895"/>
+        <c:crossAx val="1185549887"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="49872895"/>
+        <c:axId val="1185549887"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -875,7 +935,463 @@
             <a:endParaRPr lang="en-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49871935"/>
+        <c:crossAx val="1185549407"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-DK"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DK"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MeasDataNew!$K$158</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rad/s</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>MeasDataNew!$J$159:$J$166</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>MeasDataNew!$K$159:$K$166</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>-5.2928999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.5449980000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.2540259999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.793716</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.851943</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.910145999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13.333416</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6584-49E9-8C6E-3E82CD2BB586}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1185581087"/>
+        <c:axId val="1185583007"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1185581087"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="da-DK"/>
+                  <a:t>pwm(i)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DK"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1185583007"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1185583007"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="da-DK"/>
+                  <a:t>Rad/s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DK"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1185581087"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -971,6 +1487,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1487,27 +2043,543 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>257174</xdr:colOff>
-      <xdr:row>129</xdr:row>
-      <xdr:rowOff>92075</xdr:rowOff>
+      <xdr:colOff>482847</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>44780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>539749</xdr:colOff>
-      <xdr:row>144</xdr:row>
-      <xdr:rowOff>73025</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>172770</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>4701</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1C245B8-06FF-E4BA-6C42-860F5DF36C80}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35E0AC4F-69DD-826D-B45E-C07B2D26630B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1520,6 +2592,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>357798</xdr:colOff>
+      <xdr:row>154</xdr:row>
+      <xdr:rowOff>17462</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>45183</xdr:colOff>
+      <xdr:row>169</xdr:row>
+      <xdr:rowOff>13066</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E88939A7-D4C1-60D2-BD30-7659F1BAD2DB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1845,13 +2953,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB635CE0-FF05-4854-8869-C8CDB037F1F4}">
-  <dimension ref="A1:E213"/>
+  <dimension ref="A1:K213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" zoomScale="189" workbookViewId="0">
-      <selection activeCell="G149" sqref="G149"/>
+    <sheetView tabSelected="1" topLeftCell="C136" zoomScale="104" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="W151" sqref="W151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="17.6328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1">
@@ -3001,7 +4112,7 @@
         <v>13.703799</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>15587089</v>
       </c>
@@ -3009,7 +4120,7 @@
         <v>13.862527</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>15607267</v>
       </c>
@@ -3017,7 +4128,7 @@
         <v>13.862513999999999</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>15627486</v>
       </c>
@@ -3025,7 +4136,7 @@
         <v>13.862538000000001</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>15647666</v>
       </c>
@@ -3033,7 +4144,7 @@
         <v>13.22763</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>15667843</v>
       </c>
@@ -3041,7 +4152,7 @@
         <v>14.709115000000001</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>15688051</v>
       </c>
@@ -3049,7 +4160,7 @@
         <v>13.809609</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>0</v>
       </c>
@@ -3060,25 +4171,28 @@
         <v>2</v>
       </c>
       <c r="E137" t="s">
+        <v>4</v>
+      </c>
+      <c r="F137" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>13001806</v>
       </c>
       <c r="B138">
         <v>0</v>
       </c>
-      <c r="D138">
+      <c r="E138">
         <v>0</v>
       </c>
-      <c r="E138">
+      <c r="F138">
         <f>B138</f>
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>13022220</v>
       </c>
@@ -3086,11 +4200,15 @@
         <v>5.3439139999999998</v>
       </c>
       <c r="D139">
-        <f>A139/1000000000+D138</f>
-        <v>1.3022219999999999E-2</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+        <f>(A139-A138)/1000000</f>
+        <v>2.0414000000000002E-2</v>
+      </c>
+      <c r="E139">
+        <f>E138+D139</f>
+        <v>2.0414000000000002E-2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>13042425</v>
       </c>
@@ -3098,15 +4216,19 @@
         <v>4.3386459999999998</v>
       </c>
       <c r="D140">
-        <f t="shared" ref="D140:D149" si="1">A140/1000000000+D139</f>
-        <v>2.6064644999999997E-2</v>
+        <f t="shared" ref="D140:D154" si="1">(A140-A139)/1000000</f>
+        <v>2.0205000000000001E-2</v>
       </c>
       <c r="E140">
-        <f t="shared" ref="E139:E149" si="2">B140</f>
+        <f>E139+D140</f>
+        <v>4.0619000000000002E-2</v>
+      </c>
+      <c r="F140">
+        <f t="shared" ref="F140:F149" si="2">B140</f>
         <v>4.3386459999999998</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>13062613</v>
       </c>
@@ -3115,14 +4237,18 @@
       </c>
       <c r="D141">
         <f t="shared" si="1"/>
-        <v>3.9127257999999998E-2</v>
+        <v>2.0188000000000001E-2</v>
       </c>
       <c r="E141">
+        <f>E140+D141</f>
+        <v>6.0807E-2</v>
+      </c>
+      <c r="F141">
         <f t="shared" si="2"/>
         <v>6.2963009999999997</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>13082799</v>
       </c>
@@ -3131,14 +4257,18 @@
       </c>
       <c r="D142">
         <f t="shared" si="1"/>
-        <v>5.2210056999999997E-2</v>
+        <v>2.0185999999999999E-2</v>
       </c>
       <c r="E142">
+        <f>E141+D142</f>
+        <v>8.0992999999999996E-2</v>
+      </c>
+      <c r="F142">
         <f t="shared" si="2"/>
         <v>7.6190470000000001</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>13102973</v>
       </c>
@@ -3147,14 +4277,18 @@
       </c>
       <c r="D143">
         <f t="shared" si="1"/>
-        <v>6.5313029999999994E-2</v>
+        <v>2.0174000000000001E-2</v>
       </c>
       <c r="E143">
+        <f>E142+D143</f>
+        <v>0.10116699999999999</v>
+      </c>
+      <c r="F143">
         <f t="shared" si="2"/>
         <v>9.1006280000000004</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>13123160</v>
       </c>
@@ -3163,14 +4297,18 @@
       </c>
       <c r="D144">
         <f t="shared" si="1"/>
-        <v>7.8436189999999989E-2</v>
+        <v>2.0187E-2</v>
       </c>
       <c r="E144">
+        <f>E143+D144</f>
+        <v>0.12135399999999999</v>
+      </c>
+      <c r="F144">
         <f t="shared" si="2"/>
         <v>9.1006280000000004</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>13143388</v>
       </c>
@@ -3179,14 +4317,18 @@
       </c>
       <c r="D145">
         <f t="shared" si="1"/>
-        <v>9.1579577999999995E-2</v>
+        <v>2.0227999999999999E-2</v>
       </c>
       <c r="E145">
+        <f>E144+D145</f>
+        <v>0.14158199999999999</v>
+      </c>
+      <c r="F145">
         <f t="shared" si="2"/>
         <v>10.634988999999999</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>13163596</v>
       </c>
@@ -3195,14 +4337,18 @@
       </c>
       <c r="D146">
         <f t="shared" si="1"/>
-        <v>0.10474317399999999</v>
+        <v>2.0208E-2</v>
       </c>
       <c r="E146">
+        <f>E145+D146</f>
+        <v>0.16178999999999999</v>
+      </c>
+      <c r="F146">
         <f t="shared" si="2"/>
         <v>11.375737000000001</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>13183769</v>
       </c>
@@ -3211,14 +4357,18 @@
       </c>
       <c r="D147">
         <f t="shared" si="1"/>
-        <v>0.11792694299999999</v>
+        <v>2.0173E-2</v>
       </c>
       <c r="E147">
+        <f>E146+D147</f>
+        <v>0.18196299999999999</v>
+      </c>
+      <c r="F147">
         <f t="shared" si="2"/>
         <v>11.851927999999999</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>13203949</v>
       </c>
@@ -3227,14 +4377,18 @@
       </c>
       <c r="D148">
         <f t="shared" si="1"/>
-        <v>0.131130892</v>
+        <v>2.018E-2</v>
       </c>
       <c r="E148">
+        <f>E147+D148</f>
+        <v>0.20214299999999999</v>
+      </c>
+      <c r="F148">
         <f t="shared" si="2"/>
         <v>12.275218000000001</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>13224129</v>
       </c>
@@ -3243,14 +4397,18 @@
       </c>
       <c r="D149">
         <f t="shared" si="1"/>
-        <v>0.144355021</v>
+        <v>2.018E-2</v>
       </c>
       <c r="E149">
+        <f>E148+D149</f>
+        <v>0.22232299999999999</v>
+      </c>
+      <c r="F149">
         <f t="shared" si="2"/>
         <v>12.804311999999999</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>13244309</v>
       </c>
@@ -3258,15 +4416,19 @@
         <v>15.555652</v>
       </c>
       <c r="D150">
-        <f t="shared" ref="D150:D154" si="3">A150/1000000000+D149</f>
-        <v>0.15759933000000001</v>
+        <f t="shared" si="1"/>
+        <v>2.018E-2</v>
       </c>
       <c r="E150">
-        <f t="shared" ref="E150:E154" si="4">B150</f>
+        <f>E149+D150</f>
+        <v>0.242503</v>
+      </c>
+      <c r="F150">
+        <f t="shared" ref="F150:F154" si="3">B150</f>
         <v>15.555652</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>13264529</v>
       </c>
@@ -3274,15 +4436,19 @@
         <v>10.423332</v>
       </c>
       <c r="D151">
+        <f t="shared" si="1"/>
+        <v>2.0219999999999998E-2</v>
+      </c>
+      <c r="E151">
+        <f>E150+D151</f>
+        <v>0.26272299999999998</v>
+      </c>
+      <c r="F151">
         <f t="shared" si="3"/>
-        <v>0.17086385900000001</v>
-      </c>
-      <c r="E151">
-        <f t="shared" si="4"/>
         <v>10.423332</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A152">
         <v>13284710</v>
       </c>
@@ -3290,15 +4456,19 @@
         <v>13.227606</v>
       </c>
       <c r="D152">
+        <f t="shared" si="1"/>
+        <v>2.0181000000000001E-2</v>
+      </c>
+      <c r="E152">
+        <f>E151+D152</f>
+        <v>0.28290399999999999</v>
+      </c>
+      <c r="F152">
         <f t="shared" si="3"/>
-        <v>0.18414856900000001</v>
-      </c>
-      <c r="E152">
-        <f t="shared" si="4"/>
         <v>13.227606</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A153">
         <v>13304920</v>
       </c>
@@ -3306,15 +4476,19 @@
         <v>13.386321000000001</v>
       </c>
       <c r="D153">
+        <f t="shared" si="1"/>
+        <v>2.0209999999999999E-2</v>
+      </c>
+      <c r="E153">
+        <f>E152+D153</f>
+        <v>0.30311399999999999</v>
+      </c>
+      <c r="F153">
         <f t="shared" si="3"/>
-        <v>0.19745348900000001</v>
-      </c>
-      <c r="E153">
-        <f t="shared" si="4"/>
         <v>13.386321000000001</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A154">
         <v>13325100</v>
       </c>
@@ -3322,23 +4496,31 @@
         <v>13.386333</v>
       </c>
       <c r="D154">
+        <f t="shared" si="1"/>
+        <v>2.018E-2</v>
+      </c>
+      <c r="E154">
+        <f>E153+D154</f>
+        <v>0.32329399999999997</v>
+      </c>
+      <c r="F154">
         <f t="shared" si="3"/>
-        <v>0.21077858900000002</v>
-      </c>
-      <c r="E154">
-        <f t="shared" si="4"/>
         <v>13.386333</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A155">
         <v>13345278</v>
       </c>
       <c r="B155">
         <v>13.545073</v>
       </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G155">
+        <f>F154*0.63</f>
+        <v>8.4333897899999997</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A156">
         <v>13365459</v>
       </c>
@@ -3346,7 +4528,7 @@
         <v>13.703799</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>13385682</v>
       </c>
@@ -3354,79 +4536,133 @@
         <v>14.074159</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>13405861</v>
       </c>
       <c r="B158">
         <v>11.164116999999999</v>
       </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="J158" t="s">
+        <v>5</v>
+      </c>
+      <c r="K158" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>13426096</v>
       </c>
       <c r="B159">
         <v>13.650893999999999</v>
       </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="J159">
+        <v>0</v>
+      </c>
+      <c r="K159">
+        <v>-5.2928999999999997E-2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>13446272</v>
       </c>
       <c r="B160">
         <v>13.862491</v>
       </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="J160">
+        <v>0.25</v>
+      </c>
+      <c r="K160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>13466445</v>
       </c>
       <c r="B161">
         <v>15.185237000000001</v>
       </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="J161">
+        <v>0.5</v>
+      </c>
+      <c r="K161">
+        <v>3.5449980000000001</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>13486631</v>
       </c>
       <c r="B162">
         <v>13.809609</v>
       </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="J162">
+        <v>0.75</v>
+      </c>
+      <c r="K162">
+        <v>8.2540259999999996</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A163">
         <v>13506812</v>
       </c>
       <c r="B163">
         <v>11.375712999999999</v>
       </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="J163">
+        <v>1</v>
+      </c>
+      <c r="K163">
+        <v>10.793716</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A164">
         <v>13527023</v>
       </c>
       <c r="B164">
         <v>13.597918</v>
       </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="J164">
+        <v>1.25</v>
+      </c>
+      <c r="K164">
+        <v>11.851943</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A165">
         <v>13547199</v>
       </c>
       <c r="B165">
         <v>13.650893999999999</v>
       </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="J165">
+        <v>1.5</v>
+      </c>
+      <c r="K165">
+        <v>12.910145999999999</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A166">
         <v>13567373</v>
       </c>
       <c r="B166">
         <v>13.597965</v>
       </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="J166">
+        <v>1.75</v>
+      </c>
+      <c r="K166">
+        <v>13.333416</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A167">
         <v>13587545</v>
       </c>
@@ -3434,7 +4670,7 @@
         <v>13.756703999999999</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A168">
         <v>13607721</v>
       </c>
@@ -3442,7 +4678,7 @@
         <v>5.1852169999999997</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A169">
         <v>13627899</v>
       </c>
@@ -3450,7 +4686,7 @@
         <v>14.232892</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A170">
         <v>13648082</v>
       </c>
@@ -3458,7 +4694,7 @@
         <v>13.862527</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A171">
         <v>13668260</v>
       </c>
@@ -3466,7 +4702,7 @@
         <v>14.021255999999999</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A172">
         <v>13688437</v>
       </c>
@@ -3474,7 +4710,7 @@
         <v>17.777891</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A173">
         <v>13708646</v>
       </c>
@@ -3482,7 +4718,7 @@
         <v>12.539764999999999</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A174">
         <v>13728822</v>
       </c>
@@ -3490,7 +4726,7 @@
         <v>13.492144</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A175">
         <v>13749031</v>
       </c>
@@ -3498,7 +4734,7 @@
         <v>13.650893999999999</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A176">
         <v>13769208</v>
       </c>

</xml_diff>